<commit_message>
remove header line in question excel
</commit_message>
<xml_diff>
--- a/question_templates/example_questions_template.xlsx
+++ b/question_templates/example_questions_template.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jingwen/Desktop/2024Fall/AC297/AI-enabled-Index-Investing/question_templates/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65E4D57-A768-EB49-8D81-6D3D7DA43100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - question_template_per" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1 - question_template_per" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
-  <si>
-    <t>question_template_per_category</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>Category</t>
   </si>
@@ -97,26 +103,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -224,33 +223,30 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -261,26 +257,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -479,7 +534,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -497,7 +552,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -526,7 +581,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -551,7 +606,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -576,7 +631,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -601,7 +656,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -626,7 +681,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -651,7 +706,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -676,7 +731,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -701,7 +756,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -726,7 +781,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -739,9 +794,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -758,7 +819,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -776,7 +837,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -801,7 +862,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -826,7 +887,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -851,7 +912,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -876,7 +937,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -901,7 +962,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -926,7 +987,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -951,7 +1012,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -976,7 +1037,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1001,7 +1062,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1014,9 +1075,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1030,7 +1097,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1048,7 +1115,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1077,7 +1144,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1102,7 +1169,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1127,7 +1194,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1152,7 +1219,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1177,7 +1244,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1202,7 +1269,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1227,7 +1294,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1252,7 +1319,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1277,7 +1344,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1290,212 +1357,213 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:B22"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="83.3516" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="2" max="2" width="83.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+    </row>
+    <row r="2" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="4">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s" s="5">
+    </row>
+    <row r="3" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s" s="7">
+    <row r="4" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s" s="7">
+    <row r="5" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s" s="7">
+    <row r="6" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s" s="7">
+    <row r="7" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s" s="7">
+    <row r="8" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s" s="7">
+    <row r="9" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s" s="7">
+    <row r="10" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s" s="7">
+    <row r="11" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="6">
+      <c r="B11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s" s="7">
+    </row>
+    <row r="12" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s" s="7">
+    <row r="13" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s" s="7">
+    <row r="14" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s" s="7">
+    <row r="15" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" t="s" s="6">
+      <c r="B15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="s" s="7">
+    </row>
+    <row r="16" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="B17" t="s" s="7">
+    <row r="17" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" t="s" s="6">
+      <c r="B17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B18" t="s" s="7">
+    </row>
+    <row r="18" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s" s="7">
+    <row r="19" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s" s="7">
+    <row r="20" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s" s="7">
+    <row r="21" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s" s="7">
-        <v>26</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>